<commit_message>
csv import to inclide AC, not tested. started redis dev
</commit_message>
<xml_diff>
--- a/CDS JIRA.xlsx
+++ b/CDS JIRA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheahchr\git\jira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AFFED2-3907-4816-A907-6E9B3F332190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C099DB5-6628-4687-A4CB-0CC58F8CC691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14085" yWindow="9795" windowWidth="31380" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12585" yWindow="13545" windowWidth="26580" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IBDS1 flow" sheetId="5" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="178">
   <si>
     <t>Summary</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Sprint</t>
-  </si>
-  <si>
-    <t>Custom field (Epic Link)</t>
   </si>
   <si>
     <t>Issue Type</t>
@@ -1482,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F71721B-A117-46E1-B457-83694868650D}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,7 +1490,7 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -1507,63 +1504,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E2,K2)</f>
@@ -1578,80 +1575,80 @@
         <v>TWC3149</v>
       </c>
       <c r="L2" s="10" t="str">
-        <f>VLOOKUP(A2,IBDS1_AC,2,0)</f>
+        <f t="shared" ref="L2:L20" si="2">VLOOKUP(A2,IBDS1_AC,2,0)</f>
         <v>Finalize LDM with DA
 Complete PDM readiness</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E3,K3)</f>
         <v>2023.R1.2w.S1 TWC3149</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3" si="2">VLOOKUP(I3,sprints,2,0)</f>
+        <f t="shared" ref="J3" si="3">VLOOKUP(I3,sprints,2,0)</f>
         <v>181686</v>
       </c>
       <c r="K3" s="1" t="str">
-        <f t="shared" ref="K3" si="3">VLOOKUP(H3,Projects,2,0)</f>
+        <f t="shared" ref="K3" si="4">VLOOKUP(H3,Projects,2,0)</f>
         <v>TWC3149</v>
       </c>
       <c r="L3" s="10" t="str">
-        <f>VLOOKUP(A3,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">Mapping document, technical design, PDM, WIKI, test plan published and reviewed </v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="7" t="str">
-        <f t="shared" ref="I4:I17" si="4">_xlfn.TEXTJOIN(" ",1,E4,K4)</f>
+        <f t="shared" ref="I4:I17" si="5">_xlfn.TEXTJOIN(" ",1,E4,K4)</f>
         <v>2023.R1.2w.S2 TWC3149</v>
       </c>
       <c r="J4" s="1">
@@ -1663,34 +1660,34 @@
         <v>TWC3149</v>
       </c>
       <c r="L4" s="10" t="str">
-        <f>VLOOKUP(A4,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>ETL run sccessfully without error</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H5" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E5,K5)</f>
@@ -1705,37 +1702,37 @@
         <v>TWC3149</v>
       </c>
       <c r="L5" s="10" t="str">
-        <f>VLOOKUP(A5,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>ETL run sccessfully without error</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2023.R1.2w.S2 TWC4618</v>
       </c>
       <c r="J6" s="1">
@@ -1747,34 +1744,34 @@
         <v>TWC4618</v>
       </c>
       <c r="L6" s="10" t="str">
-        <f>VLOOKUP(A6,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>DB development completed and tested without error</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E7,K7)</f>
@@ -1789,35 +1786,35 @@
         <v>TWC4618</v>
       </c>
       <c r="L7" s="10" t="str">
-        <f>VLOOKUP(A7,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully
 Query view on selected rows returns valid data</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E8,K8)</f>
@@ -1832,34 +1829,34 @@
         <v>TWC3149</v>
       </c>
       <c r="L8" s="10" t="str">
-        <f>VLOOKUP(A8,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>API development completed and tested without error</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E9,K9)</f>
@@ -1874,35 +1871,35 @@
         <v>TWC3149</v>
       </c>
       <c r="L9" s="10" t="str">
-        <f>VLOOKUP(A9,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully
 Query API returns valid data</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H10" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E10,K10)</f>
@@ -1917,34 +1914,34 @@
         <v>TWC4618</v>
       </c>
       <c r="L10" s="10" t="str">
-        <f>VLOOKUP(A10,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Complete API development and unit testing</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I11" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E11,K11)</f>
@@ -1959,38 +1956,38 @@
         <v>TWC4618</v>
       </c>
       <c r="L11" s="10" t="str">
-        <f>VLOOKUP(A11,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully
 Query API returns valid data</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
         <v>7</v>
       </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
       <c r="H12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I12" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2023.R1.2w.S2 TWC4618</v>
       </c>
       <c r="J12" s="1">
@@ -2002,34 +1999,34 @@
         <v>TWC4618</v>
       </c>
       <c r="L12" s="10" t="str">
-        <f>VLOOKUP(A12,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Complete functional testing with sample data</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H13" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I13" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E13,K13)</f>
@@ -2044,35 +2041,35 @@
         <v>TWC3149</v>
       </c>
       <c r="L13" s="10" t="str">
-        <f>VLOOKUP(A13,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Batch job run successfully
 Query view on refreshed rows returns valid data</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H14" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I14" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E14,K14)</f>
@@ -2087,35 +2084,35 @@
         <v>TWC3149</v>
       </c>
       <c r="L14" s="10" t="str">
-        <f>VLOOKUP(A14,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Batch job run successfully
 Query view on refreshed rows returns valid data</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
         <v>7</v>
       </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I15" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E15,K15)</f>
@@ -2130,38 +2127,38 @@
         <v>TWC3149</v>
       </c>
       <c r="L15" s="10" t="str">
-        <f>VLOOKUP(A15,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>New/updated features work as per specification without impacting existing business scenario.
 Test cases and results documented and tracked in JIRA</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" t="s">
         <v>7</v>
       </c>
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
       <c r="H16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I16" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2023.R1.2w.S4 TWC4618</v>
       </c>
       <c r="J16" s="1">
@@ -2173,38 +2170,38 @@
         <v>TWC4618</v>
       </c>
       <c r="L16" s="10" t="str">
-        <f>VLOOKUP(A16,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Prod migration completed successfully
 Query view on selected rows returns valid data</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
         <v>7</v>
       </c>
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
       <c r="H17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2023.R1.2w.S4 TWC3149</v>
       </c>
       <c r="J17" s="1">
@@ -2216,35 +2213,35 @@
         <v>TWC3149</v>
       </c>
       <c r="L17" s="10" t="str">
-        <f>VLOOKUP(A17,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Prod migration completed successfully
 Query API returns valid data</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I18" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E18,K18)</f>
@@ -2259,35 +2256,35 @@
         <v>TWC4618</v>
       </c>
       <c r="L18" s="10" t="str">
-        <f>VLOOKUP(A18,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully
 Query API returns valid data</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H19" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="13" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E19,K19)</f>
@@ -2302,49 +2299,49 @@
         <v>TWC3149</v>
       </c>
       <c r="L19" s="10" t="str">
-        <f>VLOOKUP(A19,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>ETL run sccessfully without error</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H20" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I20" s="13" t="str">
-        <f t="shared" ref="I20" si="5">_xlfn.TEXTJOIN(" ",1,E20,K20)</f>
+        <f t="shared" ref="I20" si="6">_xlfn.TEXTJOIN(" ",1,E20,K20)</f>
         <v>2023.R1.2w.S4 TWC3149</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" ref="J20" si="6">VLOOKUP(I20,sprints,2,0)</f>
+        <f t="shared" ref="J20" si="7">VLOOKUP(I20,sprints,2,0)</f>
         <v>181707</v>
       </c>
       <c r="K20" s="10" t="str">
-        <f t="shared" ref="K20" si="7">VLOOKUP(H20,Projects,2,0)</f>
+        <f t="shared" ref="K20" si="8">VLOOKUP(H20,Projects,2,0)</f>
         <v>TWC3149</v>
       </c>
       <c r="L20" s="10" t="str">
-        <f>VLOOKUP(A20,IBDS1_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Batch job run successfully
 Query view on refreshed rows returns valid data</v>
       </c>
@@ -2377,8 +2374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,7 +2385,7 @@
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" bestFit="1" customWidth="1"/>
@@ -2402,63 +2399,63 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E2,K2)</f>
@@ -2473,35 +2470,35 @@
         <v>TWC3149</v>
       </c>
       <c r="L2" s="10" t="str">
-        <f>VLOOKUP(A2,HANA_AC,2,0)</f>
+        <f t="shared" ref="L2:L18" si="2">VLOOKUP(A2,HANA_AC,2,0)</f>
         <v>Finalize LDM with DA
 Complete PDM readiness</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E3,K3)</f>
@@ -2516,34 +2513,34 @@
         <v>TWC3149</v>
       </c>
       <c r="L3" s="10" t="str">
-        <f>VLOOKUP(A3,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Complete Mapping document, technical design, PDM, WIKI, test plan</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="7" t="str">
         <f>_xlfn.TEXTJOIN(" ",1,E4,K4)</f>
@@ -2558,37 +2555,37 @@
         <v>TWC3149</v>
       </c>
       <c r="L4" s="10" t="str">
-        <f>VLOOKUP(A4,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Complete ETL design document</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5" s="7" t="str">
-        <f t="shared" ref="I5:I18" si="2">_xlfn.TEXTJOIN(" ",1,E5,K5)</f>
+        <f t="shared" ref="I5:I18" si="3">_xlfn.TEXTJOIN(" ",1,E5,K5)</f>
         <v>2023.R1.2w.S2 TWC4618</v>
       </c>
       <c r="J5" s="1">
@@ -2600,7 +2597,7 @@
         <v>TWC4618</v>
       </c>
       <c r="L5" s="10" t="str">
-        <f>VLOOKUP(A5,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>DS job setup and tested running successfully
 Source tables visible in HANA
 New tables created</v>
@@ -2608,31 +2605,31 @@
     </row>
     <row r="6" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="9">
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H6" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S2 TWC4618</v>
       </c>
       <c r="J6" s="10">
@@ -2644,7 +2641,7 @@
         <v>TWC4618</v>
       </c>
       <c r="L6" s="10" t="str">
-        <f>VLOOKUP(A6,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>DS job setup and tested running successfully
 Source tables visible in HANA
 New tables created</v>
@@ -2652,85 +2649,85 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f t="shared" ref="I7" si="3">_xlfn.TEXTJOIN(" ",1,E7,K7)</f>
+        <f t="shared" ref="I7" si="4">_xlfn.TEXTJOIN(" ",1,E7,K7)</f>
         <v>2023.R1.2w.S2 TWC4618</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" ref="J7" si="4">VLOOKUP(I7,sprints,2,0)</f>
+        <f t="shared" ref="J7" si="5">VLOOKUP(I7,sprints,2,0)</f>
         <v>181346</v>
       </c>
       <c r="K7" s="1" t="str">
-        <f t="shared" ref="K7" si="5">VLOOKUP(H7,Projects,2,0)</f>
+        <f t="shared" ref="K7" si="6">VLOOKUP(H7,Projects,2,0)</f>
         <v>TWC4618</v>
       </c>
       <c r="L7" s="10" t="str">
-        <f>VLOOKUP(A7,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="7" t="str">
-        <f t="shared" ref="I8" si="6">_xlfn.TEXTJOIN(" ",1,E8,K8)</f>
+        <f t="shared" ref="I8" si="7">_xlfn.TEXTJOIN(" ",1,E8,K8)</f>
         <v>2023.R1.2w.S2 TWC4618</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" ref="J8" si="7">VLOOKUP(I8,sprints,2,0)</f>
+        <f t="shared" ref="J8" si="8">VLOOKUP(I8,sprints,2,0)</f>
         <v>181346</v>
       </c>
       <c r="K8" s="1" t="str">
-        <f t="shared" ref="K8" si="8">VLOOKUP(H8,Projects,2,0)</f>
+        <f t="shared" ref="K8" si="9">VLOOKUP(H8,Projects,2,0)</f>
         <v>TWC4618</v>
       </c>
       <c r="L8" s="10" t="str">
-        <f>VLOOKUP(A8,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>A,B,C,D view created/updated as per design document 
 Validate changes made not impacting other views
 Query view on selected rows returns valid data</v>
@@ -2738,31 +2735,31 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S3 TWC4618</v>
       </c>
       <c r="J9" s="1">
@@ -2774,123 +2771,123 @@
         <v>TWC4618</v>
       </c>
       <c r="L9" s="10" t="str">
-        <f>VLOOKUP(A9,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully
 Query view on selected rows returns valid data</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="7" t="str">
-        <f t="shared" ref="I10:I11" si="9">_xlfn.TEXTJOIN(" ",1,E10,K10)</f>
+        <f t="shared" ref="I10:I11" si="10">_xlfn.TEXTJOIN(" ",1,E10,K10)</f>
         <v>2023.R1.2w.S3 TWC4618</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" ref="J10:J11" si="10">VLOOKUP(I10,sprints,2,0)</f>
+        <f t="shared" ref="J10:J11" si="11">VLOOKUP(I10,sprints,2,0)</f>
         <v>181352</v>
       </c>
       <c r="K10" s="1" t="str">
-        <f t="shared" ref="K10:K11" si="11">VLOOKUP(H10,Projects,2,0)</f>
+        <f t="shared" ref="K10:K11" si="12">VLOOKUP(H10,Projects,2,0)</f>
         <v>TWC4618</v>
       </c>
       <c r="L10" s="10" t="str">
-        <f>VLOOKUP(A10,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>HANA Code developed as per IT standard</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" s="9">
         <v>1</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H11" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I11" s="13" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2023.R1.2w.S3 TWC4618</v>
       </c>
       <c r="J11" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>181352</v>
       </c>
       <c r="K11" s="10" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>TWC4618</v>
       </c>
       <c r="L11" s="10" t="str">
-        <f>VLOOKUP(A11,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Batch run successfully
 Query view on refreshed rows returns valid data</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" t="s">
         <v>7</v>
       </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
       <c r="H12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S3 TWC3149</v>
       </c>
       <c r="J12" s="1">
@@ -2902,38 +2899,38 @@
         <v>TWC3149</v>
       </c>
       <c r="L12" s="10" t="str">
-        <f>VLOOKUP(A12,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>New/updated features work as per specification without impacting existing business scenario.
 Test cases and results documented and tracked in JIRA</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" t="s">
         <v>7</v>
       </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
       <c r="H13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S3 TWC4618</v>
       </c>
       <c r="J13" s="1">
@@ -2945,37 +2942,37 @@
         <v>TWC4618</v>
       </c>
       <c r="L13" s="10" t="str">
-        <f>VLOOKUP(A13,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Complete API development and unit testing</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" t="s">
         <v>7</v>
       </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
       <c r="H14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S3 TWC4618</v>
       </c>
       <c r="J14" s="1">
@@ -2987,124 +2984,124 @@
         <v>TWC4618</v>
       </c>
       <c r="L14" s="10" t="str">
-        <f>VLOOKUP(A14,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>QA migration completed successfully
 Query API returns valid data</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" t="s">
         <v>7</v>
       </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" ref="I15" si="12">_xlfn.TEXTJOIN(" ",1,E15,K15)</f>
+        <f t="shared" ref="I15" si="13">_xlfn.TEXTJOIN(" ",1,E15,K15)</f>
         <v>2023.R1.2w.S4 TWC4618</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" ref="J15" si="13">VLOOKUP(I15,sprints,2,0)</f>
+        <f t="shared" ref="J15" si="14">VLOOKUP(I15,sprints,2,0)</f>
         <v>181366</v>
       </c>
       <c r="K15" s="1" t="str">
-        <f t="shared" ref="K15" si="14">VLOOKUP(H15,Projects,2,0)</f>
+        <f t="shared" ref="K15" si="15">VLOOKUP(H15,Projects,2,0)</f>
         <v>TWC4618</v>
       </c>
       <c r="L15" s="10" t="str">
-        <f>VLOOKUP(A15,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Prod migration completed successfully
 Query view on refreshed rows returns valid data</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="H16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I16" s="13" t="str">
-        <f t="shared" ref="I16" si="15">_xlfn.TEXTJOIN(" ",1,E16,K16)</f>
+        <f t="shared" ref="I16" si="16">_xlfn.TEXTJOIN(" ",1,E16,K16)</f>
         <v>2023.R1.2w.S4 TWC4618</v>
       </c>
       <c r="J16" s="10">
-        <f t="shared" ref="J16" si="16">VLOOKUP(I16,sprints,2,0)</f>
+        <f t="shared" ref="J16" si="17">VLOOKUP(I16,sprints,2,0)</f>
         <v>181366</v>
       </c>
       <c r="K16" s="10" t="str">
-        <f t="shared" ref="K16" si="17">VLOOKUP(H16,Projects,2,0)</f>
+        <f t="shared" ref="K16" si="18">VLOOKUP(H16,Projects,2,0)</f>
         <v>TWC4618</v>
       </c>
       <c r="L16" s="10" t="str">
-        <f>VLOOKUP(A16,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Batch run successfully
 Query view on refreshed rows returns valid data</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" t="s">
         <v>7</v>
       </c>
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
       <c r="H17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S4 TWC4618</v>
       </c>
       <c r="J17" s="1">
@@ -3116,38 +3113,38 @@
         <v>TWC4618</v>
       </c>
       <c r="L17" s="10" t="str">
-        <f>VLOOKUP(A17,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Prod migration completed successfully
 Query view on selected rows returns valid data</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
         <v>7</v>
       </c>
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
       <c r="H18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2023.R1.2w.S4 TWC3149</v>
       </c>
       <c r="J18" s="1">
@@ -3159,7 +3156,7 @@
         <v>TWC3149</v>
       </c>
       <c r="L18" s="10" t="str">
-        <f>VLOOKUP(A18,HANA_AC,2,0)</f>
+        <f t="shared" si="2"/>
         <v>Prod migration completed successfully
 Query API returns valid data</v>
       </c>
@@ -3209,344 +3206,344 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>147205</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>147207</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>147210</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>147212</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>147214</v>
       </c>
       <c r="G6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>147217</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>147220</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>160667</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>160674</v>
       </c>
       <c r="G10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>160720</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>160777</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>160802</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>160839</v>
       </c>
       <c r="G14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <v>160854</v>
       </c>
       <c r="G15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>169863</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>169871</v>
       </c>
       <c r="G17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>169887</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>169902</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>169918</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>169929</v>
       </c>
       <c r="G21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>169938</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>181686</v>
       </c>
       <c r="G23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>181695</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>181705</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>181707</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>181710</v>
       </c>
       <c r="G27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28">
         <v>181722</v>
       </c>
       <c r="G28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>181734</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30">
         <v>178762</v>
@@ -3554,7 +3551,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31">
         <v>178763</v>
@@ -3562,7 +3559,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B32">
         <v>178764</v>
@@ -3570,7 +3567,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33">
         <v>178765</v>
@@ -3578,7 +3575,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34">
         <v>178766</v>
@@ -3586,7 +3583,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35">
         <v>178767</v>
@@ -3594,7 +3591,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36">
         <v>178768</v>
@@ -3602,7 +3599,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37">
         <v>178769</v>
@@ -3610,7 +3607,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38">
         <v>178770</v>
@@ -3618,7 +3615,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39">
         <v>178771</v>
@@ -3626,7 +3623,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B40">
         <v>178772</v>
@@ -3634,7 +3631,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41">
         <v>178773</v>
@@ -3642,7 +3639,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42">
         <v>178774</v>
@@ -3650,7 +3647,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B43">
         <v>178775</v>
@@ -3658,7 +3655,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B44">
         <v>178776</v>
@@ -3666,7 +3663,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45">
         <v>181341</v>
@@ -3674,7 +3671,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B46">
         <v>181346</v>
@@ -3682,7 +3679,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B47">
         <v>181352</v>
@@ -3690,7 +3687,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B48">
         <v>181366</v>
@@ -3698,7 +3695,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B49">
         <v>181398</v>
@@ -3706,7 +3703,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50">
         <v>181421</v>
@@ -3714,7 +3711,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B51">
         <v>181478</v>
@@ -3743,163 +3740,163 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C18" s="9"/>
     </row>
@@ -3925,163 +3922,163 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -4106,79 +4103,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.use vba to call python script to refresh csv file. 2.externalize configuration 3.Use venv 4. README.md include installation steps
</commit_message>
<xml_diff>
--- a/CDS JIRA.xlsx
+++ b/CDS JIRA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cheahchr\git\jira\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C099DB5-6628-4687-A4CB-0CC58F8CC691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96490DD-8809-4C4A-89C6-AAB1BCD117B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12585" yWindow="13545" windowWidth="26580" windowHeight="15270" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3615" yWindow="4845" windowWidth="28425" windowHeight="15255" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IBDS1 flow" sheetId="5" r:id="rId1"/>
@@ -2375,7 +2375,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,19 +2626,19 @@
         <v>7</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" si="3"/>
-        <v>2023.R1.2w.S2 TWC4618</v>
+        <v>2023.R1.2w.S2 TWC3149</v>
       </c>
       <c r="J6" s="10">
         <f t="shared" si="0"/>
-        <v>181346</v>
+        <v>181695</v>
       </c>
       <c r="K6" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>TWC4618</v>
+        <v>TWC3149</v>
       </c>
       <c r="L6" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2799,19 +2799,19 @@
         <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" ref="I10:I11" si="10">_xlfn.TEXTJOIN(" ",1,E10,K10)</f>
-        <v>2023.R1.2w.S3 TWC4618</v>
+        <v>2023.R1.2w.S3 TWC3149</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" ref="J10:J11" si="11">VLOOKUP(I10,sprints,2,0)</f>
-        <v>181352</v>
+        <v>181705</v>
       </c>
       <c r="K10" s="1" t="str">
         <f t="shared" ref="K10:K11" si="12">VLOOKUP(H10,Projects,2,0)</f>
-        <v>TWC4618</v>
+        <v>TWC3149</v>
       </c>
       <c r="L10" s="10" t="str">
         <f t="shared" si="2"/>
@@ -2841,19 +2841,19 @@
         <v>7</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I11" s="13" t="str">
         <f t="shared" si="10"/>
-        <v>2023.R1.2w.S3 TWC4618</v>
+        <v>2023.R1.2w.S3 TWC3149</v>
       </c>
       <c r="J11" s="10">
         <f t="shared" si="11"/>
-        <v>181352</v>
+        <v>181705</v>
       </c>
       <c r="K11" s="10" t="str">
         <f t="shared" si="12"/>
-        <v>TWC4618</v>
+        <v>TWC3149</v>
       </c>
       <c r="L11" s="10" t="str">
         <f t="shared" si="2"/>
@@ -3055,19 +3055,19 @@
         <v>7</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I16" s="13" t="str">
         <f t="shared" ref="I16" si="16">_xlfn.TEXTJOIN(" ",1,E16,K16)</f>
-        <v>2023.R1.2w.S4 TWC4618</v>
+        <v>2023.R1.2w.S4 TWC3149</v>
       </c>
       <c r="J16" s="10">
         <f t="shared" ref="J16" si="17">VLOOKUP(I16,sprints,2,0)</f>
-        <v>181366</v>
+        <v>181707</v>
       </c>
       <c r="K16" s="10" t="str">
         <f t="shared" ref="K16" si="18">VLOOKUP(H16,Projects,2,0)</f>
-        <v>TWC4618</v>
+        <v>TWC3149</v>
       </c>
       <c r="L16" s="10" t="str">
         <f t="shared" si="2"/>
@@ -3141,19 +3141,19 @@
         <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I18" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>2023.R1.2w.S4 TWC3149</v>
+        <v>2023.R1.2w.S4 TWC4618</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="0"/>
-        <v>181707</v>
+        <v>181366</v>
       </c>
       <c r="K18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>TWC3149</v>
+        <v>TWC4618</v>
       </c>
       <c r="L18" s="10" t="str">
         <f t="shared" si="2"/>
@@ -3164,7 +3164,7 @@
   </sheetData>
   <autoFilter ref="A1:L18" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E18" xr:uid="{6E44BAF2-B077-4267-BB96-6B7ABC512781}">
       <formula1>sprint_names</formula1>
     </dataValidation>
@@ -3173,7 +3173,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9B7743FD-102E-4D74-A826-B14244B24A9F}">
           <x14:formula1>
             <xm:f>lookup!$D$2:$D$3</xm:f>

</xml_diff>